<commit_message>
Major - Update 04_
Finished!
</commit_message>
<xml_diff>
--- a/datasets/DataFrameSpreadsheet.xlsx
+++ b/datasets/DataFrameSpreadsheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="27">
   <si>
     <t>Soft</t>
   </si>
@@ -46,6 +46,9 @@
     <t>Rep</t>
   </si>
   <si>
+    <t>Prot</t>
+  </si>
+  <si>
     <t>PD</t>
   </si>
   <si>
@@ -89,6 +92,9 @@
   </si>
   <si>
     <t>R4</t>
+  </si>
+  <si>
+    <t>PEPTIDE</t>
   </si>
 </sst>
 </file>
@@ -446,13 +452,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -483,16 +489,19 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2">
         <v>1.340379708264428</v>
@@ -501,30 +510,33 @@
         <v>0.4009630088225484</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>22</v>
+      </c>
+      <c r="K2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3">
         <v>-0.9869413197284669</v>
@@ -533,30 +545,33 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>23</v>
+      </c>
+      <c r="K3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4">
         <v>1.04598747809058</v>
@@ -565,30 +580,33 @@
         <v>0.7179007099510828</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>24</v>
+      </c>
+      <c r="K4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5">
         <v>-1.345051431116523</v>
@@ -597,30 +615,33 @@
         <v>0.1387966657108421</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>25</v>
+      </c>
+      <c r="K5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6">
         <v>0.3486149815944181</v>
@@ -629,30 +650,33 @@
         <v>0.830168364402957</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>22</v>
+      </c>
+      <c r="K6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D7">
         <v>0.4799451078992153</v>
@@ -661,59 +685,65 @@
         <v>0.7876009285539736</v>
       </c>
       <c r="F7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>23</v>
+      </c>
+      <c r="K7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E8">
         <v>0.2375050246349405</v>
       </c>
       <c r="F8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <v>24</v>
+      </c>
+      <c r="K8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D9">
         <v>-1.245522790665052</v>
@@ -722,30 +752,33 @@
         <v>0.8965891495010481</v>
       </c>
       <c r="F9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+        <v>25</v>
+      </c>
+      <c r="K9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D10">
         <v>-0.1433677807023918</v>
@@ -754,30 +787,33 @@
         <v>0.2787576495636448</v>
       </c>
       <c r="F10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+        <v>22</v>
+      </c>
+      <c r="K10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D11">
         <v>-0.2883182470176846</v>
@@ -786,30 +822,33 @@
         <v>0.5573902748739504</v>
       </c>
       <c r="F11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+        <v>23</v>
+      </c>
+      <c r="K11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D12">
         <v>-0.6038003188109676</v>
@@ -818,30 +857,33 @@
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+        <v>24</v>
+      </c>
+      <c r="K12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D13">
         <v>1.39807461219245</v>
@@ -850,19 +892,22 @@
         <v>0.5887548114845748</v>
       </c>
       <c r="F13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J13" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="K13" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>